<commit_message>
Update Executor in case Special Player exists
</commit_message>
<xml_diff>
--- a/input/TrafficControl.xlsx
+++ b/input/TrafficControl.xlsx
@@ -723,7 +723,7 @@
   <dimension ref="A1:CG221"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="43"/>

</xml_diff>